<commit_message>
modificaciones en el excel de estructuras de datos
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -69,9 +69,6 @@
     <t>jugador  -&gt;</t>
   </si>
   <si>
-    <t>MAJO</t>
-  </si>
-  <si>
     <t>LEO</t>
   </si>
   <si>
@@ -169,6 +166,39 @@
   </si>
   <si>
     <t>puntaje total</t>
+  </si>
+  <si>
+    <t>lilmauro</t>
+  </si>
+  <si>
+    <t>brunardo</t>
+  </si>
+  <si>
+    <t>mermariel</t>
+  </si>
+  <si>
+    <t>fabro</t>
+  </si>
+  <si>
+    <t>fronchi</t>
+  </si>
+  <si>
+    <t>ariana</t>
+  </si>
+  <si>
+    <t>santaclau</t>
+  </si>
+  <si>
+    <t>cristeanus</t>
+  </si>
+  <si>
+    <t>torchinsky</t>
+  </si>
+  <si>
+    <t>joma</t>
+  </si>
+  <si>
+    <t>&lt;--INDICE NUMERICO</t>
   </si>
 </sst>
 </file>
@@ -292,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -330,7 +360,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -343,6 +372,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -563,7 +602,7 @@
   <dimension ref="A3:W229"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -646,7 +685,7 @@
         <v>20</v>
       </c>
       <c r="W3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -675,43 +714,43 @@
         <v>8</v>
       </c>
       <c r="J4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="R4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="S4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="U4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="9" t="s">
+      <c r="V4" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="V4" s="9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -745,8 +784,8 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -774,14 +813,28 @@
       <c r="E12" s="14">
         <v>3</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="25">
         <v>4</v>
       </c>
       <c r="G12" s="14">
         <v>5</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="H12" s="14">
+        <v>6</v>
+      </c>
+      <c r="I12" s="14">
+        <v>7</v>
+      </c>
+      <c r="J12" s="14">
+        <v>8</v>
+      </c>
+      <c r="K12" s="28">
+        <v>9</v>
+      </c>
+      <c r="L12" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12" s="27"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
@@ -793,10 +846,10 @@
       <c r="V12" s="3"/>
     </row>
     <row r="13" spans="1:23">
-      <c r="A13" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -805,65 +858,107 @@
       <c r="D13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
+      <c r="E13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
     </row>
     <row r="14" spans="1:23" ht="15" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
+      <c r="B14" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
     </row>
     <row r="15" spans="1:23" ht="15" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="16">
         <v>3</v>
       </c>
       <c r="C15" s="11">
+        <v>4</v>
+      </c>
+      <c r="D15" s="11">
+        <v>5</v>
+      </c>
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="15">
         <v>2</v>
       </c>
-      <c r="D15" s="11">
+      <c r="G15" s="15">
+        <v>6</v>
+      </c>
+      <c r="H15" s="15">
+        <v>2</v>
+      </c>
+      <c r="I15" s="15">
+        <v>2</v>
+      </c>
+      <c r="J15" s="15">
+        <v>1</v>
+      </c>
+      <c r="K15" s="15">
         <v>4</v>
       </c>
-      <c r="E15" s="15">
-        <v>5</v>
-      </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
     </row>
     <row r="16" spans="1:23" ht="15" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="11">
         <v>4</v>
@@ -872,88 +967,114 @@
         <v>5</v>
       </c>
       <c r="D16" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16" s="15">
-        <v>2</v>
-      </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-    </row>
-    <row r="18" spans="1:12" ht="15" customHeight="1">
+        <v>16</v>
+      </c>
+      <c r="F16" s="15">
+        <v>15</v>
+      </c>
+      <c r="G16" s="15">
+        <v>7</v>
+      </c>
+      <c r="H16" s="15">
+        <v>14</v>
+      </c>
+      <c r="I16" s="15">
+        <v>14</v>
+      </c>
+      <c r="J16" s="15">
+        <v>16</v>
+      </c>
+      <c r="K16" s="15">
+        <v>14</v>
+      </c>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+    </row>
+    <row r="17" spans="1:13" ht="15" customHeight="1">
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+    </row>
+    <row r="18" spans="1:13" ht="15" customHeight="1">
       <c r="B18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" customHeight="1">
+      <c r="B19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" customHeight="1">
+      <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1">
-      <c r="B19" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1">
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1">
-      <c r="B21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+    <row r="22" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="25" t="s">
-        <v>47</v>
+      <c r="C25" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="K25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="L25" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1">
-      <c r="B26" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="22">
-        <v>8</v>
-      </c>
-      <c r="E26" s="22">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B26" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="15">
+        <v>2</v>
+      </c>
+      <c r="D26" s="21">
+        <v>22</v>
+      </c>
+      <c r="E26" s="21">
         <v>2</v>
       </c>
       <c r="F26" s="10">
@@ -975,17 +1096,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="33" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="34" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="35" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="36" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B36" s="24"/>
+      <c r="B36" s="23"/>
       <c r="E36" s="7"/>
     </row>
     <row r="37" spans="2:5" ht="15.75" customHeight="1"/>

</xml_diff>